<commit_message>
script updates and clean up
</commit_message>
<xml_diff>
--- a/Automation/runs/Critical_path_OPS.xlsx
+++ b/Automation/runs/Critical_path_OPS.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3480" yWindow="3020" windowWidth="28820" windowHeight="14540" activeTab="1"/>
+    <workbookView xWindow="3480" yWindow="3020" windowWidth="28820" windowHeight="14540"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="1" r:id="rId1"/>
@@ -738,7 +738,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A13"/>
     </sheetView>
   </sheetViews>
@@ -917,7 +917,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
more updates to support dev environment
</commit_message>
<xml_diff>
--- a/Automation/runs/Critical_path_OPS.xlsx
+++ b/Automation/runs/Critical_path_OPS.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3480" yWindow="3020" windowWidth="28820" windowHeight="14540"/>
+    <workbookView xWindow="3480" yWindow="3000" windowWidth="28820" windowHeight="14540" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="1" r:id="rId1"/>
@@ -212,13 +212,13 @@
     <t>threadCount</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
     <t>remote</t>
   </si>
   <si>
     <t>1400x1050</t>
+  </si>
+  <si>
+    <t>4</t>
   </si>
 </sst>
 </file>
@@ -738,7 +738,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="A4" sqref="A2:A13"/>
     </sheetView>
   </sheetViews>
@@ -917,8 +917,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -942,7 +942,7 @@
         <v>13</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -974,7 +974,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -1049,7 +1049,7 @@
         <v>56</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
fixes for dev runs and added implicitewait param to the excel
</commit_message>
<xml_diff>
--- a/Automation/runs/Critical_path_OPS.xlsx
+++ b/Automation/runs/Critical_path_OPS.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="15960" windowHeight="18080" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="63">
   <si>
     <t>Execute</t>
   </si>
@@ -184,6 +184,7 @@
         <sz val="11"/>
         <color indexed="17"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>vahan+qa@heal.com</t>
     </r>
@@ -220,6 +221,12 @@
   </si>
   <si>
     <t>prod</t>
+  </si>
+  <si>
+    <t>implicitWait</t>
+  </si>
+  <si>
+    <t>30</t>
   </si>
 </sst>
 </file>
@@ -237,18 +244,21 @@
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color indexed="9"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color indexed="17"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1697,7 +1707,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A14"/>
     </sheetView>
   </sheetViews>
@@ -1927,7 +1937,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -2107,8 +2117,12 @@
       <c r="E15" s="7"/>
     </row>
     <row r="16" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="4"/>
-      <c r="B16" s="7"/>
+      <c r="A16" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>62</v>
+      </c>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>

</xml_diff>

<commit_message>
added update patient API
</commit_message>
<xml_diff>
--- a/Automation/runs/Critical_path_OPS.xlsx
+++ b/Automation/runs/Critical_path_OPS.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="64">
   <si>
     <t>Execute</t>
   </si>
@@ -227,6 +227,9 @@
   </si>
   <si>
     <t>30</t>
+  </si>
+  <si>
+    <t>addInsuranceToVisit</t>
   </si>
 </sst>
 </file>
@@ -1705,10 +1708,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A2" sqref="A2:A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1923,6 +1926,20 @@
       </c>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
+    </row>
+    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="7"/>
+      <c r="D15" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
created new OpsAPI to handle visit cleanups and more
</commit_message>
<xml_diff>
--- a/Automation/runs/Critical_path_OPS.xlsx
+++ b/Automation/runs/Critical_path_OPS.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28702"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="41180" windowHeight="18080"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18080"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="1" r:id="rId1"/>
@@ -211,9 +211,6 @@
     <t>N</t>
   </si>
   <si>
-    <t>Regression</t>
-  </si>
-  <si>
     <t>critical</t>
   </si>
   <si>
@@ -239,6 +236,9 @@
   </si>
   <si>
     <t>refundVisitTotal</t>
+  </si>
+  <si>
+    <t>regression</t>
   </si>
 </sst>
 </file>
@@ -1774,7 +1774,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A4" sqref="A2:A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1809,7 +1809,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="20" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="18" t="s">
@@ -1823,7 +1823,7 @@
       <c r="F2" s="19"/>
     </row>
     <row r="3" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="20" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="21" t="s">
@@ -1837,7 +1837,7 @@
       <c r="F3" s="22"/>
     </row>
     <row r="4" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="20" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="21" t="s">
@@ -1851,7 +1851,7 @@
       <c r="F4" s="22"/>
     </row>
     <row r="5" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="20" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="21" t="s">
@@ -1859,13 +1859,13 @@
       </c>
       <c r="C5" s="19"/>
       <c r="D5" s="21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E5" s="22"/>
       <c r="F5" s="22"/>
     </row>
     <row r="6" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="20" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="21" t="s">
@@ -1873,13 +1873,13 @@
       </c>
       <c r="C6" s="19"/>
       <c r="D6" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E6" s="22"/>
       <c r="F6" s="22"/>
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="20" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="21" t="s">
@@ -1887,13 +1887,13 @@
       </c>
       <c r="C7" s="19"/>
       <c r="D7" s="21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E7" s="22"/>
       <c r="F7" s="22"/>
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="20" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="21" t="s">
@@ -1901,13 +1901,13 @@
       </c>
       <c r="C8" s="19"/>
       <c r="D8" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E8" s="22"/>
       <c r="F8" s="22"/>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="20" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="21" t="s">
@@ -1921,7 +1921,7 @@
       <c r="F9" s="22"/>
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="20" t="s">
         <v>6</v>
       </c>
       <c r="B10" s="21" t="s">
@@ -1929,13 +1929,13 @@
       </c>
       <c r="C10" s="19"/>
       <c r="D10" s="21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E10" s="22"/>
       <c r="F10" s="22"/>
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="20" t="s">
         <v>6</v>
       </c>
       <c r="B11" s="21" t="s">
@@ -1943,13 +1943,13 @@
       </c>
       <c r="C11" s="19"/>
       <c r="D11" s="21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E11" s="22"/>
       <c r="F11" s="22"/>
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="20" t="s">
         <v>6</v>
       </c>
       <c r="B12" s="21" t="s">
@@ -1957,13 +1957,13 @@
       </c>
       <c r="C12" s="19"/>
       <c r="D12" s="21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E12" s="22"/>
       <c r="F12" s="22"/>
     </row>
     <row r="13" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="20" t="s">
         <v>6</v>
       </c>
       <c r="B13" s="21" t="s">
@@ -1977,7 +1977,7 @@
       <c r="F13" s="22"/>
     </row>
     <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="20" t="s">
         <v>6</v>
       </c>
       <c r="B14" s="21" t="s">
@@ -1985,7 +1985,7 @@
       </c>
       <c r="C14" s="19"/>
       <c r="D14" s="21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E14" s="22"/>
       <c r="F14" s="22"/>
@@ -1998,7 +1998,7 @@
         <v>13</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="D15" s="21" t="s">
         <v>17</v>
@@ -2014,7 +2014,7 @@
         <v>7</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>8</v>
@@ -2030,7 +2030,7 @@
         <v>9</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>10</v>
@@ -2046,7 +2046,7 @@
         <v>11</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>12</v>
@@ -2062,7 +2062,7 @@
         <v>13</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>14</v>
@@ -2078,7 +2078,7 @@
         <v>15</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>16</v>

</xml_diff>